<commit_message>
debugging lure hit fish.
</commit_message>
<xml_diff>
--- a/config/xlsx/tool.xlsx
+++ b/config/xlsx/tool.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17535" activeTab="1"/>
+    <workbookView windowWidth="29535" windowHeight="17535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
     <sheet name="HookToolParam" sheetId="2" r:id="rId2"/>
+    <sheet name="backlog" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="64">
   <si>
     <t>约定说明</t>
   </si>
@@ -156,6 +157,21 @@
   </si>
   <si>
     <t>segment</t>
+  </si>
+  <si>
+    <t>Ogle_Lake</t>
+  </si>
+  <si>
+    <t>lure_minnow03_4</t>
+  </si>
+  <si>
+    <t>[鱼饵运动类型]抽搐</t>
+  </si>
+  <si>
+    <t>[地图水层]中层</t>
+  </si>
+  <si>
+    <t>[水下结构体]断层</t>
   </si>
   <si>
     <t>ROBloodwormFloatGrass200-13</t>
@@ -306,21 +322,9 @@
     <t>[水下结构体]泥底</t>
   </si>
   <si>
-    <t>Ogle_Lake</t>
-  </si>
-  <si>
-    <t>lure_minnow03_4</t>
-  </si>
-  <si>
     <t>[鱼饵运动类型]直走摇晃</t>
   </si>
   <si>
-    <t>[地图水层]中层</t>
-  </si>
-  <si>
-    <t>[水下结构体]断层</t>
-  </si>
-  <si>
     <t>[鱼饵运动类型]自由落体</t>
   </si>
   <si>
@@ -328,9 +332,6 @@
   </si>
   <si>
     <t>[鱼饵运动类型]摇晃</t>
-  </si>
-  <si>
-    <t>[鱼饵运动类型]抽搐</t>
   </si>
   <si>
     <t>[鱼饵运动类型]停走</t>
@@ -1115,10 +1116,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1164,6 +1161,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1559,8 +1560,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="37.575" style="20" customWidth="1"/>
-    <col min="2" max="2" width="20.8583333333333" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.575" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.8583333333333" style="19" customWidth="1"/>
+    <col min="3" max="3" width="44.575" style="19" customWidth="1"/>
     <col min="4" max="4" width="20.575" style="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1630,10 +1631,10 @@
       <c r="A11" s="30">
         <v>45735</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1648,1512 +1649,1710 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="18.575" style="18" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="23.2916666666667" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.0083333333333" style="19" customWidth="1"/>
+    <col min="5" max="5" width="21.8583333333333" style="19" customWidth="1"/>
+    <col min="6" max="6" width="13.2916666666667" style="18" customWidth="1"/>
+    <col min="7" max="7" width="31.2916666666667" style="19" customWidth="1"/>
+    <col min="8" max="8" width="21.375" style="19" customWidth="1"/>
+    <col min="9" max="9" width="17.8583333333333" style="18" customWidth="1"/>
+    <col min="10" max="10" width="14.2916666666667" style="18" customWidth="1"/>
+    <col min="11" max="11" width="11.2916666666667" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="19.5" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1" spans="1:11">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" ht="33" customHeight="1" spans="1:11">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1" spans="1:11">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="12">
+        <v>9</v>
+      </c>
+      <c r="B5" s="13" t="str">
+        <f>_xlfn.CONCAT("minnow",RIGHT(E5,4),RIGHT(G5,4),RIGHT(H5,4))</f>
+        <v>minnow型]抽搐层]中层体]断层</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="12">
+        <v>100</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12">
+        <v>180</v>
+      </c>
+      <c r="J5" s="12">
+        <v>15</v>
+      </c>
+      <c r="K5" s="12">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C5" errorStyle="warning">
+      <formula1>COUNTIF($A:$A,C5)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="D5" errorStyle="warning">
+      <formula1>COUNTIF($G:$G,D5)&lt;2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="18.575" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.2916666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.0083333333333" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.8583333333333" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.2916666666667" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.2916666666667" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.8583333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.2916666666667" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.2916666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="10.125" customWidth="1"/>
+    <col min="7" max="7" width="29.125" customWidth="1"/>
+    <col min="8" max="8" width="21.375" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="12.875" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="15" spans="1:11">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1" spans="1:11">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="15" spans="1:11">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" ht="33" customHeight="1" spans="1:11">
-      <c r="A3" s="7" t="s">
+    <row r="3" ht="43.5" spans="1:11">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" ht="19.5" customHeight="1" spans="1:11">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
+    <row r="4" ht="15" spans="1:11">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" ht="15" spans="1:11">
-      <c r="A5" s="11">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="11">
-        <v>100</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="9">
+        <v>100</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="9">
+        <v>200</v>
+      </c>
+      <c r="J5" s="9">
+        <v>13</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:11">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="9">
+        <v>100</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="9">
+        <v>220</v>
+      </c>
+      <c r="J6" s="9">
+        <v>15</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:11">
+      <c r="A7" s="12">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="12">
+        <v>100</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="12">
+        <v>160</v>
+      </c>
+      <c r="J7" s="12">
+        <v>15</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:11">
+      <c r="A8" s="9">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="str">
+        <f t="shared" ref="B8:B42" si="0">_xlfn.CONCAT("minnow",RIGHT(E8,4),RIGHT(G8,4),RIGHT(H8,4))</f>
+        <v>minnow直走摇晃层]中层体]断层</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="12">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="11">
-        <v>200</v>
-      </c>
-      <c r="J5" s="11">
-        <v>13</v>
-      </c>
-      <c r="K5" s="14">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" ht="15" spans="1:11">
-      <c r="A6" s="11">
-        <v>2</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="11">
-        <v>100</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="11">
-        <v>220</v>
-      </c>
-      <c r="J6" s="11">
-        <v>15</v>
-      </c>
-      <c r="K6" s="14">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" ht="15" spans="1:11">
-      <c r="A7" s="14">
-        <v>3</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="14">
-        <v>100</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="14">
-        <v>160</v>
-      </c>
-      <c r="J7" s="14">
-        <v>15</v>
-      </c>
-      <c r="K7" s="14">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" ht="15" spans="1:11">
-      <c r="A8" s="11">
-        <v>4</v>
-      </c>
-      <c r="B8" s="15" t="str">
-        <f>_xlfn.CONCAT("minnow",RIGHT(E8,4),RIGHT(G8,4),RIGHT(H8,4))</f>
-        <v>minnow直走摇晃层]中层体]断层</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="14">
-        <v>100</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="14">
-        <v>180</v>
-      </c>
-      <c r="J8" s="14">
-        <v>15</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1000</v>
+      <c r="I8" s="12">
+        <v>180</v>
+      </c>
+      <c r="J8" s="12">
+        <v>15</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:11">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="15" t="str">
-        <f t="shared" ref="B9:B42" si="0">_xlfn.CONCAT("minnow",RIGHT(E9,4),RIGHT(G9,4),RIGHT(H9,4))</f>
+      <c r="B9" s="13" t="str">
+        <f t="shared" si="0"/>
         <v>minnow自由落体层]中层体]断层</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="14">
-        <v>100</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="14">
-        <v>180</v>
-      </c>
-      <c r="J9" s="14">
-        <v>15</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1000</v>
+      <c r="C9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="12">
+        <v>100</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="12">
+        <v>180</v>
+      </c>
+      <c r="J9" s="12">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="14">
+      <c r="A10" s="12">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="str">
+      <c r="B10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]直走层]中层体]断层</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="14">
-        <v>100</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="14">
-        <v>180</v>
-      </c>
-      <c r="J10" s="14">
-        <v>15</v>
-      </c>
-      <c r="K10" s="14">
-        <v>1000</v>
+      <c r="C10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="12">
+        <v>100</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="12">
+        <v>180</v>
+      </c>
+      <c r="J10" s="12">
+        <v>15</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:11">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="str">
+      <c r="B11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]断层</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="14">
-        <v>100</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="14">
-        <v>180</v>
-      </c>
-      <c r="J11" s="14">
-        <v>15</v>
-      </c>
-      <c r="K11" s="14">
-        <v>1000</v>
+      <c r="C11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="12">
+        <v>100</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="12">
+        <v>180</v>
+      </c>
+      <c r="J11" s="12">
+        <v>15</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:11">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="str">
+      <c r="B12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]摇晃层]中层体]断层</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="14">
-        <v>100</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="14">
-        <v>180</v>
-      </c>
-      <c r="J12" s="14">
-        <v>15</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1000</v>
+      <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="12">
+        <v>100</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="12">
+        <v>180</v>
+      </c>
+      <c r="J12" s="12">
+        <v>15</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="14">
+      <c r="A13" s="12">
         <v>9</v>
       </c>
-      <c r="B13" s="15" t="str">
+      <c r="B13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]抽搐层]中层体]断层</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="14">
-        <v>100</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="14">
-        <v>180</v>
-      </c>
-      <c r="J13" s="14">
-        <v>15</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1000</v>
+      <c r="C13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="12">
+        <v>100</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="12">
+        <v>180</v>
+      </c>
+      <c r="J13" s="12">
+        <v>15</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:11">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="15" t="str">
+      <c r="B14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]停走层]中层体]断层</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="C14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="14">
-        <v>100</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="14">
-        <v>180</v>
-      </c>
-      <c r="J14" s="14">
-        <v>15</v>
-      </c>
-      <c r="K14" s="14">
-        <v>1000</v>
+      <c r="F14" s="12">
+        <v>100</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="12">
+        <v>180</v>
+      </c>
+      <c r="J14" s="12">
+        <v>15</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:11">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="15" t="str">
+      <c r="B15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层开放水域</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="14">
-        <v>100</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="17" t="s">
+      <c r="C15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="12">
+        <v>100</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="14">
-        <v>180</v>
-      </c>
-      <c r="J15" s="14">
-        <v>15</v>
-      </c>
-      <c r="K15" s="14">
-        <v>1000</v>
+      <c r="I15" s="12">
+        <v>180</v>
+      </c>
+      <c r="J15" s="12">
+        <v>15</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="14">
+      <c r="A16" s="12">
         <v>12</v>
       </c>
-      <c r="B16" s="15" t="str">
+      <c r="B16" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow自由落体层]中层开放水域</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="14">
-        <v>100</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="17" t="s">
+      <c r="C16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="12">
+        <v>100</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="14">
-        <v>180</v>
-      </c>
-      <c r="J16" s="14">
-        <v>15</v>
-      </c>
-      <c r="K16" s="14">
-        <v>1000</v>
+      <c r="I16" s="12">
+        <v>180</v>
+      </c>
+      <c r="J16" s="12">
+        <v>15</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:11">
-      <c r="A17" s="11">
+      <c r="A17" s="9">
         <v>13</v>
       </c>
-      <c r="B17" s="15" t="str">
+      <c r="B17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]直走层]中层开放水域</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="14">
-        <v>100</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="17" t="s">
+      <c r="C17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="12">
+        <v>100</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="14">
-        <v>180</v>
-      </c>
-      <c r="J17" s="14">
-        <v>15</v>
-      </c>
-      <c r="K17" s="14">
-        <v>1000</v>
+      <c r="I17" s="12">
+        <v>180</v>
+      </c>
+      <c r="J17" s="12">
+        <v>15</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:11">
-      <c r="A18" s="11">
+      <c r="A18" s="9">
         <v>14</v>
       </c>
-      <c r="B18" s="15" t="str">
+      <c r="B18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层开放水域</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="14">
-        <v>100</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="17" t="s">
+      <c r="C18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="12">
+        <v>100</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="14">
-        <v>180</v>
-      </c>
-      <c r="J18" s="14">
-        <v>15</v>
-      </c>
-      <c r="K18" s="14">
-        <v>1000</v>
+      <c r="I18" s="12">
+        <v>180</v>
+      </c>
+      <c r="J18" s="12">
+        <v>15</v>
+      </c>
+      <c r="K18" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="14">
-        <v>15</v>
-      </c>
-      <c r="B19" s="15" t="str">
+      <c r="A19" s="12">
+        <v>15</v>
+      </c>
+      <c r="B19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]摇晃层]中层开放水域</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="14">
-        <v>100</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="17" t="s">
+      <c r="C19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="12">
+        <v>100</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="14">
-        <v>180</v>
-      </c>
-      <c r="J19" s="14">
-        <v>15</v>
-      </c>
-      <c r="K19" s="14">
-        <v>1000</v>
+      <c r="I19" s="12">
+        <v>180</v>
+      </c>
+      <c r="J19" s="12">
+        <v>15</v>
+      </c>
+      <c r="K19" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:11">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <v>16</v>
       </c>
-      <c r="B20" s="15" t="str">
+      <c r="B20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]抽搐层]中层开放水域</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="14">
-        <v>100</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="17" t="s">
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="12">
+        <v>100</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I20" s="14">
-        <v>180</v>
-      </c>
-      <c r="J20" s="14">
-        <v>15</v>
-      </c>
-      <c r="K20" s="14">
-        <v>1000</v>
+      <c r="I20" s="12">
+        <v>180</v>
+      </c>
+      <c r="J20" s="12">
+        <v>15</v>
+      </c>
+      <c r="K20" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:11">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>17</v>
       </c>
-      <c r="B21" s="15" t="str">
+      <c r="B21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]停走层]中层开放水域</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="C21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="14">
-        <v>100</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="17" t="s">
+      <c r="F21" s="12">
+        <v>100</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="14">
-        <v>180</v>
-      </c>
-      <c r="J21" s="14">
-        <v>15</v>
-      </c>
-      <c r="K21" s="14">
-        <v>1000</v>
+      <c r="I21" s="12">
+        <v>180</v>
+      </c>
+      <c r="J21" s="12">
+        <v>15</v>
+      </c>
+      <c r="K21" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="14">
+      <c r="A22" s="12">
         <v>18</v>
       </c>
-      <c r="B22" s="15" t="str">
+      <c r="B22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]水草</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="14">
-        <v>100</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="14">
-        <v>180</v>
-      </c>
-      <c r="J22" s="14">
-        <v>15</v>
-      </c>
-      <c r="K22" s="14">
-        <v>1000</v>
+      <c r="C22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="12">
+        <v>100</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="12">
+        <v>180</v>
+      </c>
+      <c r="J22" s="12">
+        <v>15</v>
+      </c>
+      <c r="K22" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:11">
-      <c r="A23" s="11">
+      <c r="A23" s="9">
         <v>19</v>
       </c>
-      <c r="B23" s="15" t="str">
+      <c r="B23" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow自由落体层]中层体]水草</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="14">
-        <v>100</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="14">
-        <v>180</v>
-      </c>
-      <c r="J23" s="14">
-        <v>15</v>
-      </c>
-      <c r="K23" s="14">
-        <v>1000</v>
+      <c r="C23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="12">
+        <v>100</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="12">
+        <v>180</v>
+      </c>
+      <c r="J23" s="12">
+        <v>15</v>
+      </c>
+      <c r="K23" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:11">
-      <c r="A24" s="11">
+      <c r="A24" s="9">
         <v>20</v>
       </c>
-      <c r="B24" s="15" t="str">
+      <c r="B24" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]直走层]中层体]水草</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="14">
-        <v>100</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="14">
-        <v>180</v>
-      </c>
-      <c r="J24" s="14">
-        <v>15</v>
-      </c>
-      <c r="K24" s="14">
-        <v>1000</v>
+      <c r="C24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="12">
+        <v>100</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="12">
+        <v>180</v>
+      </c>
+      <c r="J24" s="12">
+        <v>15</v>
+      </c>
+      <c r="K24" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="14">
+      <c r="A25" s="12">
         <v>21</v>
       </c>
-      <c r="B25" s="15" t="str">
+      <c r="B25" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]水草</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="14">
-        <v>100</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" s="14">
-        <v>180</v>
-      </c>
-      <c r="J25" s="14">
-        <v>15</v>
-      </c>
-      <c r="K25" s="14">
-        <v>1000</v>
+      <c r="C25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="12">
+        <v>100</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="12">
+        <v>180</v>
+      </c>
+      <c r="J25" s="12">
+        <v>15</v>
+      </c>
+      <c r="K25" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:11">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <v>22</v>
       </c>
-      <c r="B26" s="15" t="str">
+      <c r="B26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]摇晃层]中层体]水草</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="14">
-        <v>100</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="14">
-        <v>180</v>
-      </c>
-      <c r="J26" s="14">
-        <v>15</v>
-      </c>
-      <c r="K26" s="14">
-        <v>1000</v>
+      <c r="C26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="12">
+        <v>100</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="12">
+        <v>180</v>
+      </c>
+      <c r="J26" s="12">
+        <v>15</v>
+      </c>
+      <c r="K26" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:11">
-      <c r="A27" s="11">
+      <c r="A27" s="9">
         <v>23</v>
       </c>
-      <c r="B27" s="15" t="str">
+      <c r="B27" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]抽搐层]中层体]水草</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="14">
-        <v>100</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="14">
-        <v>180</v>
-      </c>
-      <c r="J27" s="14">
-        <v>15</v>
-      </c>
-      <c r="K27" s="14">
-        <v>1000</v>
+      <c r="C27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="12">
+        <v>100</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="12">
+        <v>180</v>
+      </c>
+      <c r="J27" s="12">
+        <v>15</v>
+      </c>
+      <c r="K27" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="14">
+      <c r="A28" s="12">
         <v>24</v>
       </c>
-      <c r="B28" s="15" t="str">
+      <c r="B28" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]停走层]中层体]水草</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="C28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="14">
-        <v>100</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I28" s="14">
-        <v>180</v>
-      </c>
-      <c r="J28" s="14">
-        <v>15</v>
-      </c>
-      <c r="K28" s="14">
-        <v>1000</v>
+      <c r="F28" s="12">
+        <v>100</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="12">
+        <v>180</v>
+      </c>
+      <c r="J28" s="12">
+        <v>15</v>
+      </c>
+      <c r="K28" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:11">
-      <c r="A29" s="11">
+      <c r="A29" s="9">
         <v>25</v>
       </c>
-      <c r="B29" s="15" t="str">
+      <c r="B29" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]尖脊</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="14">
-        <v>100</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="17" t="s">
+      <c r="C29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="12">
+        <v>100</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="14">
-        <v>180</v>
-      </c>
-      <c r="J29" s="14">
-        <v>15</v>
-      </c>
-      <c r="K29" s="14">
-        <v>1000</v>
+      <c r="I29" s="12">
+        <v>180</v>
+      </c>
+      <c r="J29" s="12">
+        <v>15</v>
+      </c>
+      <c r="K29" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:11">
-      <c r="A30" s="11">
+      <c r="A30" s="9">
         <v>26</v>
       </c>
-      <c r="B30" s="15" t="str">
+      <c r="B30" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow自由落体层]中层体]尖脊</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="14">
-        <v>100</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="17" t="s">
+      <c r="C30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="12">
+        <v>100</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="14">
-        <v>180</v>
-      </c>
-      <c r="J30" s="14">
-        <v>15</v>
-      </c>
-      <c r="K30" s="14">
-        <v>1000</v>
+      <c r="I30" s="12">
+        <v>180</v>
+      </c>
+      <c r="J30" s="12">
+        <v>15</v>
+      </c>
+      <c r="K30" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="14">
+      <c r="A31" s="12">
         <v>27</v>
       </c>
-      <c r="B31" s="15" t="str">
+      <c r="B31" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]直走层]中层体]尖脊</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="14">
-        <v>100</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" s="17" t="s">
+      <c r="C31" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="12">
+        <v>100</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I31" s="14">
-        <v>180</v>
-      </c>
-      <c r="J31" s="14">
-        <v>15</v>
-      </c>
-      <c r="K31" s="14">
-        <v>1000</v>
+      <c r="I31" s="12">
+        <v>180</v>
+      </c>
+      <c r="J31" s="12">
+        <v>15</v>
+      </c>
+      <c r="K31" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:11">
-      <c r="A32" s="11">
+      <c r="A32" s="9">
         <v>28</v>
       </c>
-      <c r="B32" s="15" t="str">
+      <c r="B32" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]尖脊</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="14">
-        <v>100</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="17" t="s">
+      <c r="C32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="12">
+        <v>100</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="14">
-        <v>180</v>
-      </c>
-      <c r="J32" s="14">
-        <v>15</v>
-      </c>
-      <c r="K32" s="14">
-        <v>1000</v>
+      <c r="I32" s="12">
+        <v>180</v>
+      </c>
+      <c r="J32" s="12">
+        <v>15</v>
+      </c>
+      <c r="K32" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:11">
-      <c r="A33" s="11">
+      <c r="A33" s="9">
         <v>29</v>
       </c>
-      <c r="B33" s="15" t="str">
+      <c r="B33" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]摇晃层]中层体]尖脊</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="14">
-        <v>100</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" s="17" t="s">
+      <c r="C33" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="12">
+        <v>100</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="14">
-        <v>180</v>
-      </c>
-      <c r="J33" s="14">
-        <v>15</v>
-      </c>
-      <c r="K33" s="14">
-        <v>1000</v>
+      <c r="I33" s="12">
+        <v>180</v>
+      </c>
+      <c r="J33" s="12">
+        <v>15</v>
+      </c>
+      <c r="K33" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="14">
+      <c r="A34" s="12">
         <v>30</v>
       </c>
-      <c r="B34" s="15" t="str">
+      <c r="B34" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]抽搐层]中层体]尖脊</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="14">
-        <v>100</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H34" s="17" t="s">
+      <c r="C34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="12">
+        <v>100</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="14">
-        <v>180</v>
-      </c>
-      <c r="J34" s="14">
-        <v>15</v>
-      </c>
-      <c r="K34" s="14">
-        <v>1000</v>
+      <c r="I34" s="12">
+        <v>180</v>
+      </c>
+      <c r="J34" s="12">
+        <v>15</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:11">
-      <c r="A35" s="11">
+      <c r="A35" s="9">
         <v>31</v>
       </c>
-      <c r="B35" s="15" t="str">
+      <c r="B35" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]停走层]中层体]尖脊</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="17" t="s">
+      <c r="C35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="14">
-        <v>100</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H35" s="17" t="s">
+      <c r="F35" s="12">
+        <v>100</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I35" s="14">
-        <v>180</v>
-      </c>
-      <c r="J35" s="14">
-        <v>15</v>
-      </c>
-      <c r="K35" s="14">
-        <v>1000</v>
+      <c r="I35" s="12">
+        <v>180</v>
+      </c>
+      <c r="J35" s="12">
+        <v>15</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:11">
-      <c r="A36" s="11">
+      <c r="A36" s="9">
         <v>32</v>
       </c>
-      <c r="B36" s="15" t="str">
+      <c r="B36" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]岩架</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="14">
-        <v>100</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H36" s="17" t="s">
+      <c r="C36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="12">
+        <v>100</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="14">
-        <v>180</v>
-      </c>
-      <c r="J36" s="14">
-        <v>15</v>
-      </c>
-      <c r="K36" s="14">
-        <v>1000</v>
+      <c r="I36" s="12">
+        <v>180</v>
+      </c>
+      <c r="J36" s="12">
+        <v>15</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="14">
+      <c r="A37" s="12">
         <v>33</v>
       </c>
-      <c r="B37" s="15" t="str">
+      <c r="B37" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow自由落体层]中层体]岩架</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="14">
-        <v>100</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H37" s="17" t="s">
+      <c r="C37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="12">
+        <v>100</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I37" s="14">
-        <v>180</v>
-      </c>
-      <c r="J37" s="14">
-        <v>15</v>
-      </c>
-      <c r="K37" s="14">
-        <v>1000</v>
+      <c r="I37" s="12">
+        <v>180</v>
+      </c>
+      <c r="J37" s="12">
+        <v>15</v>
+      </c>
+      <c r="K37" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:11">
-      <c r="A38" s="11">
+      <c r="A38" s="9">
         <v>34</v>
       </c>
-      <c r="B38" s="15" t="str">
+      <c r="B38" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]直走层]中层体]岩架</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="14">
-        <v>100</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H38" s="17" t="s">
+      <c r="C38" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="12">
+        <v>100</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="14">
-        <v>180</v>
-      </c>
-      <c r="J38" s="14">
-        <v>15</v>
-      </c>
-      <c r="K38" s="14">
-        <v>1000</v>
+      <c r="I38" s="12">
+        <v>180</v>
+      </c>
+      <c r="J38" s="12">
+        <v>15</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:11">
-      <c r="A39" s="11">
+      <c r="A39" s="9">
         <v>35</v>
       </c>
-      <c r="B39" s="15" t="str">
+      <c r="B39" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow直走摇晃层]中层体]岩架</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="14">
-        <v>100</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H39" s="17" t="s">
+      <c r="C39" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="12">
+        <v>100</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I39" s="14">
-        <v>180</v>
-      </c>
-      <c r="J39" s="14">
-        <v>15</v>
-      </c>
-      <c r="K39" s="14">
-        <v>1000</v>
+      <c r="I39" s="12">
+        <v>180</v>
+      </c>
+      <c r="J39" s="12">
+        <v>15</v>
+      </c>
+      <c r="K39" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="14">
+      <c r="A40" s="12">
         <v>36</v>
       </c>
-      <c r="B40" s="15" t="str">
+      <c r="B40" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]摇晃层]中层体]岩架</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="14">
-        <v>100</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H40" s="17" t="s">
+      <c r="C40" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="12">
+        <v>100</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="14">
-        <v>180</v>
-      </c>
-      <c r="J40" s="14">
-        <v>15</v>
-      </c>
-      <c r="K40" s="14">
-        <v>1000</v>
+      <c r="I40" s="12">
+        <v>180</v>
+      </c>
+      <c r="J40" s="12">
+        <v>15</v>
+      </c>
+      <c r="K40" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:11">
-      <c r="A41" s="11">
-        <v>37</v>
-      </c>
-      <c r="B41" s="15" t="str">
+      <c r="A41" s="9">
+        <v>37</v>
+      </c>
+      <c r="B41" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]抽搐层]中层体]岩架</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="14">
-        <v>100</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H41" s="17" t="s">
+      <c r="C41" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="12">
+        <v>100</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="14">
-        <v>180</v>
-      </c>
-      <c r="J41" s="14">
-        <v>15</v>
-      </c>
-      <c r="K41" s="14">
-        <v>1000</v>
+      <c r="I41" s="12">
+        <v>180</v>
+      </c>
+      <c r="J41" s="12">
+        <v>15</v>
+      </c>
+      <c r="K41" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:11">
-      <c r="A42" s="11">
-        <v>38</v>
-      </c>
-      <c r="B42" s="15" t="str">
+      <c r="A42" s="9">
+        <v>38</v>
+      </c>
+      <c r="B42" s="13" t="str">
         <f t="shared" si="0"/>
         <v>minnow型]停走层]中层体]岩架</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" s="17" t="s">
+      <c r="C42" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="14">
-        <v>100</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" s="17" t="s">
+      <c r="F42" s="12">
+        <v>100</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="14">
-        <v>180</v>
-      </c>
-      <c r="J42" s="14">
-        <v>15</v>
-      </c>
-      <c r="K42" s="14">
-        <v>1000</v>
+      <c r="I42" s="12">
+        <v>180</v>
+      </c>
+      <c r="J42" s="12">
+        <v>15</v>
+      </c>
+      <c r="K42" s="12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3177,7 +3376,7 @@
       <formula1>COUNTIF($A:$A,C5)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated conf, and updated pose affs
</commit_message>
<xml_diff>
--- a/config/xlsx/tool.xlsx
+++ b/config/xlsx/tool.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17535" activeTab="2"/>
+    <workbookView windowHeight="17535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="62">
   <si>
     <t>约定说明</t>
   </si>
@@ -159,21 +159,6 @@
     <t>segment</t>
   </si>
   <si>
-    <t>Ogle_Lake</t>
-  </si>
-  <si>
-    <t>lure_minnow03_4</t>
-  </si>
-  <si>
-    <t>[鱼饵运动类型]抽搐</t>
-  </si>
-  <si>
-    <t>[地图水层]中层</t>
-  </si>
-  <si>
-    <t>[水下结构体]断层</t>
-  </si>
-  <si>
     <t>Noob_Lake</t>
   </si>
   <si>
@@ -192,13 +177,7 @@
     <t>[水下结构体]开放水域</t>
   </si>
   <si>
-    <t>ROBloodwormFloatGrass200-13</t>
-  </si>
-  <si>
     <t>bait_bloodworm</t>
-  </si>
-  <si>
-    <t>RoFishcubeFloatGrassTopMid220-15</t>
   </si>
   <si>
     <t>bait_fish_cube_1</t>
@@ -278,9 +257,6 @@
     </r>
   </si>
   <si>
-    <t>RoNibletFloatMudBottom100-15</t>
-  </si>
-  <si>
     <t>bait_niblet</t>
   </si>
   <si>
@@ -328,9 +304,21 @@
     <t>[水下结构体]泥底</t>
   </si>
   <si>
+    <t>Ogle_Lake</t>
+  </si>
+  <si>
+    <t>lure_minnow03_4</t>
+  </si>
+  <si>
     <t>[鱼饵运动类型]直走摇晃</t>
   </si>
   <si>
+    <t>[地图水层]中层</t>
+  </si>
+  <si>
+    <t>[水下结构体]断层</t>
+  </si>
+  <si>
     <t>[鱼饵运动类型]自由落体</t>
   </si>
   <si>
@@ -338,6 +326,9 @@
   </si>
   <si>
     <t>[鱼饵运动类型]摇晃</t>
+  </si>
+  <si>
+    <t>[鱼饵运动类型]抽搐</t>
   </si>
   <si>
     <t>[鱼饵运动类型]停走</t>
@@ -1666,13 +1657,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="18.575" style="22" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="23" customWidth="1"/>
@@ -1809,51 +1800,501 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="19">
-        <v>9</v>
+    <row r="5" ht="15" spans="1:11">
+      <c r="A5" s="11">
+        <v>100</v>
       </c>
       <c r="B5" s="12" t="str">
-        <f>_xlfn.CONCAT("minnow",RIGHT(E5,4),RIGHT(G5,4),RIGHT(H5,4))</f>
-        <v>minnow型]抽搐层]中层体]断层</v>
+        <f t="shared" ref="B5:B10" si="0">_xlfn.CONCAT(LEFT(C5,5),RIGHT(D5,LEN(D5)-5),RIGHT(E5,2),RIGHT(G5,2),RIGHT(H5,2),I5)</f>
+        <v>Noob_bread_1静止中层水草200</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="19">
-        <v>100</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="11">
+        <v>100</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="19">
-        <v>180</v>
-      </c>
-      <c r="J5" s="19">
-        <v>15</v>
-      </c>
-      <c r="K5" s="19">
+      <c r="I5" s="11">
+        <v>200</v>
+      </c>
+      <c r="J5" s="11">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:11">
+      <c r="A6" s="16">
+        <v>101</v>
+      </c>
+      <c r="B6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noob_bread_1静止中层水域200</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="11">
+        <v>100</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="11">
+        <v>200</v>
+      </c>
+      <c r="J6" s="11">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:11">
+      <c r="A7" s="11">
+        <v>102</v>
+      </c>
+      <c r="B7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noob_bloodworm静止中层水草200</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="16">
+        <v>100</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="16">
+        <v>200</v>
+      </c>
+      <c r="J7" s="16">
+        <v>13</v>
+      </c>
+      <c r="K7" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:11">
+      <c r="A8" s="16">
+        <v>103</v>
+      </c>
+      <c r="B8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noob_fish_cube_1静止中层水草220</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="16">
+        <v>100</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="16">
+        <v>220</v>
+      </c>
+      <c r="J8" s="16">
+        <v>15</v>
+      </c>
+      <c r="K8" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:11">
+      <c r="A9" s="11">
+        <v>104</v>
+      </c>
+      <c r="B9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noob_niblet静止底层泥底160</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="19">
+        <v>100</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="19">
+        <v>160</v>
+      </c>
+      <c r="J9" s="19">
+        <v>15</v>
+      </c>
+      <c r="K9" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:11">
+      <c r="A10" s="16">
+        <v>105</v>
+      </c>
+      <c r="B10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noob_niblet静止底层泥底120</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="19">
+        <v>100</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="19">
+        <v>120</v>
+      </c>
+      <c r="J10" s="19">
+        <v>15</v>
+      </c>
+      <c r="K10" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:11">
+      <c r="A11" s="16">
+        <v>601</v>
+      </c>
+      <c r="B11" s="12" t="str">
+        <f t="shared" ref="B11:B17" si="1">_xlfn.CONCAT(LEFT(C11,5),RIGHT(D11,LEN(D11)-5),RIGHT(E11,2),RIGHT(G11,2),RIGHT(H11,2))</f>
+        <v>Ogle_minnow03_4摇晃中层断层</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="19">
+        <v>100</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="19">
+        <v>180</v>
+      </c>
+      <c r="J11" s="19">
+        <v>15</v>
+      </c>
+      <c r="K11" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:11">
+      <c r="A12" s="16">
+        <v>602</v>
+      </c>
+      <c r="B12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4落体中层断层</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="19">
+        <v>100</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="19">
+        <v>180</v>
+      </c>
+      <c r="J12" s="19">
+        <v>15</v>
+      </c>
+      <c r="K12" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:11">
+      <c r="A13" s="16">
+        <v>603</v>
+      </c>
+      <c r="B13" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4直走中层断层</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="19">
+        <v>100</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="19">
+        <v>180</v>
+      </c>
+      <c r="J13" s="19">
+        <v>15</v>
+      </c>
+      <c r="K13" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:11">
+      <c r="A14" s="16">
+        <v>604</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4摇晃中层断层</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="19">
+        <v>100</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="19">
+        <v>180</v>
+      </c>
+      <c r="J14" s="19">
+        <v>15</v>
+      </c>
+      <c r="K14" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:11">
+      <c r="A15" s="16">
+        <v>605</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4摇晃中层断层</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="19">
+        <v>100</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="19">
+        <v>180</v>
+      </c>
+      <c r="J15" s="19">
+        <v>15</v>
+      </c>
+      <c r="K15" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:11">
+      <c r="A16" s="16">
+        <v>606</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4抽搐中层断层</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="19">
+        <v>100</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="19">
+        <v>180</v>
+      </c>
+      <c r="J16" s="19">
+        <v>15</v>
+      </c>
+      <c r="K16" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:11">
+      <c r="A17" s="16">
+        <v>607</v>
+      </c>
+      <c r="B17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ogle_minnow03_4停走中层断层</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="19">
+        <v>100</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="19">
+        <v>180</v>
+      </c>
+      <c r="J17" s="19">
+        <v>15</v>
+      </c>
+      <c r="K17" s="11">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C17">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C5" errorStyle="warning">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C5 C6 C7 C10 C8:C9 C11:C17" errorStyle="warning">
       <formula1>COUNTIF($A:$A,C5)&lt;2</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="D5" errorStyle="warning">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="D5 D6 D9 D10 D11:D17" errorStyle="warning">
       <formula1>COUNTIF($G:$G,D5)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1865,10 +2306,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="A6:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2025,26 +2466,26 @@
         <v>100</v>
       </c>
       <c r="B6" s="12" t="str">
-        <f t="shared" ref="B6:B11" si="0">_xlfn.CONCAT(LEFT(C6,5),RIGHT(D6,LEN(D6)-5),RIGHT(E6,2),RIGHT(G6,2),RIGHT(H6,2))</f>
-        <v>Noob_bread_1静止中层水草</v>
+        <f>_xlfn.CONCAT(LEFT(C6,5),RIGHT(D6,LEN(D6)-5),RIGHT(E6,2),RIGHT(G6,2),RIGHT(H6,2),I6)</f>
+        <v>Noob_bread_1静止中层水草200</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F6" s="11">
         <v>100</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I6" s="11">
         <v>200</v>
@@ -2061,26 +2502,26 @@
         <v>101</v>
       </c>
       <c r="B7" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noob_bread_1静止中层水域</v>
+        <f>_xlfn.CONCAT(LEFT(C7,5),RIGHT(D7,LEN(D7)-5),RIGHT(E7,2),RIGHT(G7,2),RIGHT(H7,2),I7)</f>
+        <v>Noob_bread_1静止中层水域200</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="11">
+        <v>100</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="11">
-        <v>100</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="I7" s="11">
         <v>200</v>
@@ -2096,26 +2537,27 @@
       <c r="A8" s="11">
         <v>102</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>48</v>
+      <c r="B8" s="12" t="str">
+        <f>_xlfn.CONCAT(LEFT(C8,5),RIGHT(D8,LEN(D8)-5),RIGHT(E8,2),RIGHT(G8,2),RIGHT(H8,2),I8)</f>
+        <v>Noob_bloodworm静止中层水草200</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F8" s="16">
         <v>100</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I8" s="16">
         <v>200</v>
@@ -2131,26 +2573,27 @@
       <c r="A9" s="16">
         <v>103</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>50</v>
+      <c r="B9" s="12" t="str">
+        <f>_xlfn.CONCAT(LEFT(C9,5),RIGHT(D9,LEN(D9)-5),RIGHT(E9,2),RIGHT(G9,2),RIGHT(H9,2),I9)</f>
+        <v>Noob_fish_cube_1静止中层水草220</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F9" s="16">
         <v>100</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I9" s="16">
         <v>220</v>
@@ -2166,26 +2609,27 @@
       <c r="A10" s="11">
         <v>104</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>53</v>
+      <c r="B10" s="12" t="str">
+        <f>_xlfn.CONCAT(LEFT(C10,5),RIGHT(D10,LEN(D10)-5),RIGHT(E10,2),RIGHT(G10,2),RIGHT(H10,2),I10)</f>
+        <v>Noob_niblet静止底层泥底160</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F10" s="19">
         <v>100</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I10" s="19">
         <v>160</v>
@@ -2199,173 +2643,173 @@
     </row>
     <row r="11" ht="15" spans="1:11">
       <c r="A11" s="16">
+        <v>105</v>
+      </c>
+      <c r="B11" s="12" t="str">
+        <f>_xlfn.CONCAT(LEFT(C11,5),RIGHT(D11,LEN(D11)-5),RIGHT(E11,2),RIGHT(G11,2),RIGHT(H11,2),I11)</f>
+        <v>Noob_niblet静止底层泥底120</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="19">
+        <v>100</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="19">
+        <v>120</v>
+      </c>
+      <c r="J11" s="19">
+        <v>15</v>
+      </c>
+      <c r="K11" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:11">
+      <c r="A12" s="16">
         <v>601</v>
       </c>
-      <c r="B11" s="12" t="str">
+      <c r="B12" s="12" t="str">
+        <f>_xlfn.CONCAT(LEFT(C12,5),RIGHT(D12,LEN(D12)-5),RIGHT(E12,2),RIGHT(G12,2),RIGHT(H12,2))</f>
+        <v>Ogle_minnow03_4摇晃中层断层</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="19">
+        <v>100</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="19">
+        <v>180</v>
+      </c>
+      <c r="J12" s="19">
+        <v>15</v>
+      </c>
+      <c r="K12" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:11">
+      <c r="A13" s="16">
+        <v>602</v>
+      </c>
+      <c r="B13" s="12" t="str">
+        <f t="shared" ref="B13:B46" si="0">_xlfn.CONCAT(LEFT(C13,5),RIGHT(D13,LEN(D13)-5),RIGHT(E13,2),RIGHT(G13,2),RIGHT(H13,2))</f>
+        <v>Ogle_minnow03_4落体中层断层</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="19">
+        <v>100</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="19">
+        <v>180</v>
+      </c>
+      <c r="J13" s="19">
+        <v>15</v>
+      </c>
+      <c r="K13" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:11">
+      <c r="A14" s="16">
+        <v>603</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4直走中层断层</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="19">
+        <v>100</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="19">
+        <v>180</v>
+      </c>
+      <c r="J14" s="19">
+        <v>15</v>
+      </c>
+      <c r="K14" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:11">
+      <c r="A15" s="16">
+        <v>604</v>
+      </c>
+      <c r="B15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Ogle_minnow03_4摇晃中层断层</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="19">
-        <v>100</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="19">
-        <v>180</v>
-      </c>
-      <c r="J11" s="19">
-        <v>15</v>
-      </c>
-      <c r="K11" s="11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" ht="15" spans="1:11">
-      <c r="A12" s="16">
-        <v>602</v>
-      </c>
-      <c r="B12" s="12" t="str">
-        <f t="shared" ref="B12:B45" si="1">_xlfn.CONCAT(LEFT(C12,5),RIGHT(D12,LEN(D12)-5),RIGHT(E12,2),RIGHT(G12,2),RIGHT(H12,2))</f>
-        <v>Ogle_minnow03_4落体中层断层</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="19">
-        <v>100</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="19">
-        <v>180</v>
-      </c>
-      <c r="J12" s="19">
-        <v>15</v>
-      </c>
-      <c r="K12" s="11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" ht="15" spans="1:11">
-      <c r="A13" s="16">
-        <v>603</v>
-      </c>
-      <c r="B13" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4直走中层断层</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="19">
-        <v>100</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="19">
-        <v>180</v>
-      </c>
-      <c r="J13" s="19">
-        <v>15</v>
-      </c>
-      <c r="K13" s="11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" ht="15" spans="1:11">
-      <c r="A14" s="16">
-        <v>604</v>
-      </c>
-      <c r="B14" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层断层</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="19">
-        <v>100</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="19">
-        <v>180</v>
-      </c>
-      <c r="J14" s="19">
-        <v>15</v>
-      </c>
-      <c r="K14" s="11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="15" ht="15" spans="1:11">
-      <c r="A15" s="16">
-        <v>605</v>
-      </c>
-      <c r="B15" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层断层</v>
-      </c>
       <c r="C15" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F15" s="19">
         <v>100</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="I15" s="19">
         <v>180</v>
@@ -2379,29 +2823,29 @@
     </row>
     <row r="16" ht="15" spans="1:11">
       <c r="A16" s="16">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4抽搐中层断层</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层断层</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F16" s="19">
         <v>100</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="I16" s="19">
         <v>180</v>
@@ -2415,29 +2859,29 @@
     </row>
     <row r="17" ht="15" spans="1:11">
       <c r="A17" s="16">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4停走中层断层</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4抽搐中层断层</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="19">
         <v>100</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="I17" s="19">
         <v>180</v>
@@ -2451,29 +2895,29 @@
     </row>
     <row r="18" ht="15" spans="1:11">
       <c r="A18" s="16">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B18" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4停走中层断层</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="F18" s="19">
         <v>100</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I18" s="19">
         <v>180</v>
@@ -2487,29 +2931,29 @@
     </row>
     <row r="19" ht="15" spans="1:11">
       <c r="A19" s="16">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B19" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4落体中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层水域</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F19" s="19">
         <v>100</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I19" s="19">
         <v>180</v>
@@ -2523,29 +2967,29 @@
     </row>
     <row r="20" ht="15" spans="1:11">
       <c r="A20" s="16">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B20" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4直走中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4落体中层水域</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F20" s="19">
         <v>100</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I20" s="19">
         <v>180</v>
@@ -2559,29 +3003,29 @@
     </row>
     <row r="21" ht="15" spans="1:11">
       <c r="A21" s="16">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B21" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4直走中层水域</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" s="19">
         <v>100</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I21" s="19">
         <v>180</v>
@@ -2595,29 +3039,29 @@
     </row>
     <row r="22" ht="15" spans="1:11">
       <c r="A22" s="16">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B22" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Ogle_minnow03_4摇晃中层水域</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F22" s="19">
         <v>100</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I22" s="19">
         <v>180</v>
@@ -2631,29 +3075,29 @@
     </row>
     <row r="23" ht="15" spans="1:11">
       <c r="A23" s="16">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B23" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4抽搐中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层水域</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F23" s="19">
         <v>100</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I23" s="19">
         <v>180</v>
@@ -2667,29 +3111,29 @@
     </row>
     <row r="24" ht="15" spans="1:11">
       <c r="A24" s="16">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B24" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4停走中层水域</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4抽搐中层水域</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F24" s="19">
         <v>100</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I24" s="19">
         <v>180</v>
@@ -2703,29 +3147,29 @@
     </row>
     <row r="25" ht="15" spans="1:11">
       <c r="A25" s="16">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B25" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4停走中层水域</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="F25" s="19">
         <v>100</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I25" s="19">
         <v>180</v>
@@ -2739,29 +3183,29 @@
     </row>
     <row r="26" ht="15" spans="1:11">
       <c r="A26" s="16">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B26" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4落体中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层水草</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F26" s="19">
         <v>100</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I26" s="19">
         <v>180</v>
@@ -2775,29 +3219,29 @@
     </row>
     <row r="27" ht="15" spans="1:11">
       <c r="A27" s="16">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B27" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4直走中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4落体中层水草</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F27" s="19">
         <v>100</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I27" s="19">
         <v>180</v>
@@ -2811,29 +3255,29 @@
     </row>
     <row r="28" ht="15" spans="1:11">
       <c r="A28" s="16">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B28" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4直走中层水草</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F28" s="19">
         <v>100</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I28" s="19">
         <v>180</v>
@@ -2847,29 +3291,29 @@
     </row>
     <row r="29" ht="15" spans="1:11">
       <c r="A29" s="16">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B29" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Ogle_minnow03_4摇晃中层水草</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F29" s="19">
         <v>100</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I29" s="19">
         <v>180</v>
@@ -2883,29 +3327,29 @@
     </row>
     <row r="30" ht="15" spans="1:11">
       <c r="A30" s="16">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B30" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4抽搐中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层水草</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F30" s="19">
         <v>100</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I30" s="19">
         <v>180</v>
@@ -2919,29 +3363,29 @@
     </row>
     <row r="31" ht="15" spans="1:11">
       <c r="A31" s="16">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B31" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4停走中层水草</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4抽搐中层水草</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F31" s="19">
         <v>100</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I31" s="19">
         <v>180</v>
@@ -2955,29 +3399,29 @@
     </row>
     <row r="32" ht="15" spans="1:11">
       <c r="A32" s="16">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B32" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4停走中层水草</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="F32" s="19">
         <v>100</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="I32" s="19">
         <v>180</v>
@@ -2991,29 +3435,29 @@
     </row>
     <row r="33" ht="15" spans="1:11">
       <c r="A33" s="16">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B33" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4落体中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层尖脊</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F33" s="19">
         <v>100</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I33" s="19">
         <v>180</v>
@@ -3027,29 +3471,29 @@
     </row>
     <row r="34" ht="15" spans="1:11">
       <c r="A34" s="16">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B34" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4直走中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4落体中层尖脊</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E34" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="19">
+        <v>100</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F34" s="19">
-        <v>100</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="I34" s="19">
         <v>180</v>
@@ -3063,29 +3507,29 @@
     </row>
     <row r="35" ht="15" spans="1:11">
       <c r="A35" s="16">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B35" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4直走中层尖脊</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" s="19">
         <v>100</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I35" s="19">
         <v>180</v>
@@ -3099,29 +3543,29 @@
     </row>
     <row r="36" ht="15" spans="1:11">
       <c r="A36" s="16">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B36" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Ogle_minnow03_4摇晃中层尖脊</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F36" s="19">
         <v>100</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I36" s="19">
         <v>180</v>
@@ -3135,29 +3579,29 @@
     </row>
     <row r="37" ht="15" spans="1:11">
       <c r="A37" s="16">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B37" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4抽搐中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层尖脊</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F37" s="19">
         <v>100</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I37" s="19">
         <v>180</v>
@@ -3171,29 +3615,29 @@
     </row>
     <row r="38" ht="15" spans="1:11">
       <c r="A38" s="16">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B38" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4停走中层尖脊</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4抽搐中层尖脊</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F38" s="19">
         <v>100</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I38" s="19">
         <v>180</v>
@@ -3207,29 +3651,29 @@
     </row>
     <row r="39" ht="15" spans="1:11">
       <c r="A39" s="16">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B39" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层岩架</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4停走中层尖脊</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="F39" s="19">
         <v>100</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I39" s="19">
         <v>180</v>
@@ -3243,29 +3687,29 @@
     </row>
     <row r="40" ht="15" spans="1:11">
       <c r="A40" s="16">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B40" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4落体中层岩架</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层岩架</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F40" s="19">
         <v>100</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I40" s="19">
         <v>180</v>
@@ -3279,29 +3723,29 @@
     </row>
     <row r="41" ht="15" spans="1:11">
       <c r="A41" s="16">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B41" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4直走中层岩架</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4落体中层岩架</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F41" s="19">
         <v>100</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I41" s="19">
         <v>180</v>
@@ -3315,29 +3759,29 @@
     </row>
     <row r="42" ht="15" spans="1:11">
       <c r="A42" s="16">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B42" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4摇晃中层岩架</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4直走中层岩架</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F42" s="19">
         <v>100</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I42" s="19">
         <v>180</v>
@@ -3351,29 +3795,29 @@
     </row>
     <row r="43" ht="15" spans="1:11">
       <c r="A43" s="16">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B43" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Ogle_minnow03_4摇晃中层岩架</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E43" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="19">
+        <v>100</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="F43" s="19">
-        <v>100</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="I43" s="19">
         <v>180</v>
@@ -3387,29 +3831,29 @@
     </row>
     <row r="44" ht="15" spans="1:11">
       <c r="A44" s="16">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B44" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Ogle_minnow03_4抽搐中层岩架</v>
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4摇晃中层岩架</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F44" s="19">
         <v>100</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I44" s="19">
         <v>180</v>
@@ -3423,64 +3867,103 @@
     </row>
     <row r="45" ht="15" spans="1:11">
       <c r="A45" s="16">
+        <v>634</v>
+      </c>
+      <c r="B45" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Ogle_minnow03_4抽搐中层岩架</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="19">
+        <v>100</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" s="19">
+        <v>180</v>
+      </c>
+      <c r="J45" s="19">
+        <v>15</v>
+      </c>
+      <c r="K45" s="11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="46" ht="15" spans="1:11">
+      <c r="A46" s="16">
         <v>635</v>
       </c>
-      <c r="B45" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="B46" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>Ogle_minnow03_4停走中层岩架</v>
       </c>
-      <c r="C45" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="19">
-        <v>100</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I45" s="19">
-        <v>180</v>
-      </c>
-      <c r="J45" s="19">
-        <v>15</v>
-      </c>
-      <c r="K45" s="11">
+      <c r="C46" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="19">
+        <v>100</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I46" s="19">
+        <v>180</v>
+      </c>
+      <c r="J46" s="19">
+        <v>15</v>
+      </c>
+      <c r="K46" s="11">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+  <conditionalFormatting sqref="C8">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C45">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="C12:C46">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C6 C7 C8 C9:C10 C11:C45" errorStyle="warning">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C6 C7 C8 C11 C9:C10 C12:C46" errorStyle="warning">
       <formula1>COUNTIF($A:$A,C6)&lt;2</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="D6 D7 D10 D11:D45" errorStyle="warning">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="D6 D7 D10 D11 D12:D46" errorStyle="warning">
       <formula1>COUNTIF($G:$G,D6)&lt;2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>